<commit_message>
Implement AI flow refactor, env-locked workbook, gameplay UX and theme updates
</commit_message>
<xml_diff>
--- a/docs/chicken-vaults.xlsx
+++ b/docs/chicken-vaults.xlsx
@@ -1,47 +1,46 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <workbookPr codeName="ThisWorkbook"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet name="TEMPLATE" sheetId="1" r:id="rId1"/>
+    <sheet sheetId="1" name="P01_Ava" state="visible" r:id="rId4"/>
+    <sheet sheetId="2" name="P02_Bo" state="visible" r:id="rId5"/>
+    <sheet sheetId="3" name="P03_Cy" state="visible" r:id="rId6"/>
   </sheets>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="5">
+  <si>
+    <t>Round</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Suits</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Level</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
-    <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
-  </numFmts>
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -65,13 +64,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -396,20 +403,1060 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E300"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="str">
-        <v>Chicken Vault template - backend will initialize player sheets</v>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
       </c>
     </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="275" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="277" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="2:5" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1"/>
-  </ignoredErrors>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Color" error="Select RED or BLACK from the dropdown." sqref="B10:B300">
+      <formula1>"RED,BLACK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Color" error="Select RED or BLACK from the dropdown." sqref="B2:B300">
+      <formula1>"RED,BLACK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Suits" error="Select S, H, D, or C from the dropdown." sqref="C10:C300">
+      <formula1>"S,H,D,C"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Suits" error="Select S, H, D, or C from the dropdown." sqref="C2:C300">
+      <formula1>"S,H,D,C"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Select an exact card code (e.g., 8S, QD) from the dropdown." sqref="D10:D300">
+      <formula1>"AS,AH,AD,AC,2S,2H,2D,2C,3S,3H,3D,3C,4S,4H,4D,4C,5S,5H,5D,5C,6S,6H,6D,6C,7S,7H,7D,7C,8S,8H,8D,8C,9S,9H,9D,9C,TS,TH,TD,TC,JS,JH,JD,JC,QS,QH,QD,QC,KS,KH,KD,KC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Select an exact card code (e.g., 8S, QD) from the dropdown." sqref="D2:D300">
+      <formula1>"AS,AH,AD,AC,2S,2H,2D,2C,3S,3H,3D,3C,4S,4H,4D,4C,5S,5H,5D,5C,6S,6H,6D,6C,7S,7H,7D,7C,8S,8H,8D,8C,9S,9H,9D,9C,TS,TH,TD,TC,JS,JH,JD,JC,QS,QH,QD,QC,KS,KH,KD,KC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Level" error="Select SAFE, MEDIUM, or BOLD from the dropdown." sqref="E10:E300">
+      <formula1>"SAFE,MEDIUM,BOLD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Level" error="Select SAFE, MEDIUM, or BOLD from the dropdown." sqref="E2:E300">
+      <formula1>"SAFE,MEDIUM,BOLD"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E300"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="275" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="277" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="2:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Color" error="Select RED or BLACK from the dropdown." sqref="B10:B300">
+      <formula1>"RED,BLACK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Color" error="Select RED or BLACK from the dropdown." sqref="B2:B300">
+      <formula1>"RED,BLACK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Suits" error="Select S, H, D, or C from the dropdown." sqref="C10:C300">
+      <formula1>"S,H,D,C"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Suits" error="Select S, H, D, or C from the dropdown." sqref="C2:C300">
+      <formula1>"S,H,D,C"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Select an exact card code (e.g., 8S, QD) from the dropdown." sqref="D10:D300">
+      <formula1>"AS,AH,AD,AC,2S,2H,2D,2C,3S,3H,3D,3C,4S,4H,4D,4C,5S,5H,5D,5C,6S,6H,6D,6C,7S,7H,7D,7C,8S,8H,8D,8C,9S,9H,9D,9C,TS,TH,TD,TC,JS,JH,JD,JC,QS,QH,QD,QC,KS,KH,KD,KC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Select an exact card code (e.g., 8S, QD) from the dropdown." sqref="D2:D300">
+      <formula1>"AS,AH,AD,AC,2S,2H,2D,2C,3S,3H,3D,3C,4S,4H,4D,4C,5S,5H,5D,5C,6S,6H,6D,6C,7S,7H,7D,7C,8S,8H,8D,8C,9S,9H,9D,9C,TS,TH,TD,TC,JS,JH,JD,JC,QS,QH,QD,QC,KS,KH,KD,KC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Level" error="Select SAFE, MEDIUM, or BOLD from the dropdown." sqref="E10:E300">
+      <formula1>"SAFE,MEDIUM,BOLD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Level" error="Select SAFE, MEDIUM, or BOLD from the dropdown." sqref="E2:E300">
+      <formula1>"SAFE,MEDIUM,BOLD"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E300"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="65" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="81" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="82" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="84" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="85" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="86" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="87" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="88" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="89" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="90" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="91" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="92" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="93" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="94" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="95" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="96" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="97" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="98" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="99" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="100" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="101" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="102" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="103" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="104" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="105" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="106" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="107" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="108" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="109" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="110" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="111" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="112" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="113" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="114" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="115" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="116" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="117" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="118" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="119" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="120" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="121" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="122" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="123" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="124" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="125" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="126" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="127" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="128" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="129" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="130" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="131" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="132" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="133" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="134" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="135" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="136" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="137" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="138" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="139" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="140" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="141" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="142" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="143" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="144" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="145" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="146" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="147" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="148" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="149" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="150" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="151" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="152" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="153" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="154" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="155" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="156" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="157" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="158" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="159" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="160" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="161" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="162" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="163" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="164" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="165" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="166" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="167" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="168" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="169" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="170" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="171" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="172" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="173" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="174" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="175" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="176" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="177" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="178" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="179" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="180" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="181" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="182" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="183" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="184" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="185" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="186" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="187" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="188" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="189" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="190" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="191" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="192" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="193" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="194" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="195" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="196" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="197" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="198" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="199" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="200" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="201" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="202" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="203" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="204" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="205" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="206" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="207" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="208" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="209" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="210" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="211" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="212" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="213" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="214" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="215" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="216" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="217" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="218" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="219" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="220" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="221" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="222" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="223" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="224" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="225" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="226" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="227" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="228" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="229" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="230" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="231" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="232" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="233" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="234" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="235" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="236" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="237" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="238" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="239" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="240" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="241" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="242" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="243" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="244" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="245" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="246" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="247" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="248" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="249" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="250" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="251" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="252" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="253" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="254" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="255" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="256" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="257" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="258" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="259" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="260" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="261" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="262" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="263" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="264" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="265" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="266" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="267" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="268" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="269" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="270" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="271" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="272" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="273" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="274" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="275" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="276" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="277" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="278" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="279" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="280" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="281" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="282" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="283" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="284" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="285" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="286" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="287" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="288" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="289" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="290" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="291" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="292" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="293" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="294" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="295" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="296" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="297" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="298" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="299" spans="2:5" x14ac:dyDescent="0.25"/>
+    <row r="300" spans="2:5" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <dataValidations count="8">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Color" error="Select RED or BLACK from the dropdown." sqref="B10:B300">
+      <formula1>"RED,BLACK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Color" error="Select RED or BLACK from the dropdown." sqref="B2:B300">
+      <formula1>"RED,BLACK"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Suits" error="Select S, H, D, or C from the dropdown." sqref="C10:C300">
+      <formula1>"S,H,D,C"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Suits" error="Select S, H, D, or C from the dropdown." sqref="C2:C300">
+      <formula1>"S,H,D,C"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Select an exact card code (e.g., 8S, QD) from the dropdown." sqref="D10:D300">
+      <formula1>"AS,AH,AD,AC,2S,2H,2D,2C,3S,3H,3D,3C,4S,4H,4D,4C,5S,5H,5D,5C,6S,6H,6D,6C,7S,7H,7D,7C,8S,8H,8D,8C,9S,9H,9D,9C,TS,TH,TD,TC,JS,JH,JD,JC,QS,QH,QD,QC,KS,KH,KD,KC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Number" error="Select an exact card code (e.g., 8S, QD) from the dropdown." sqref="D2:D300">
+      <formula1>"AS,AH,AD,AC,2S,2H,2D,2C,3S,3H,3D,3C,4S,4H,4D,4C,5S,5H,5D,5C,6S,6H,6D,6C,7S,7H,7D,7C,8S,8H,8D,8C,9S,9H,9D,9C,TS,TH,TD,TC,JS,JH,JD,JC,QS,QH,QD,QC,KS,KH,KD,KC"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Level" error="Select SAFE, MEDIUM, or BOLD from the dropdown." sqref="E10:E300">
+      <formula1>"SAFE,MEDIUM,BOLD"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Level" error="Select SAFE, MEDIUM, or BOLD from the dropdown." sqref="E2:E300">
+      <formula1>"SAFE,MEDIUM,BOLD"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>